<commit_message>
implemented class successful for autostockin
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C45EFB4-F0BC-41C5-853D-DFEC7997CB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B1B13D-8A8F-4493-85BF-98561DFA2A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="3015" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18060" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="แปะหน้า" sheetId="1" r:id="rId1"/>
@@ -330,7 +330,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +344,14 @@
       <color theme="1"/>
       <name val="barcode font"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -353,7 +361,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -403,19 +411,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -488,25 +483,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -515,14 +504,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,113 +873,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="0.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="0.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="57" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="36.75" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="57" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="36.75" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="37.5" customHeight="1">
+      <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="70" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1027,604 +1012,604 @@
     </row>
     <row r="2" spans="1:9" ht="21.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="15" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="9"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="6.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="21.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="15" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="13" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="21.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="9"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="9" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="21.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="15" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="13" t="s">
         <v>2</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="21.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="9" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="21.75" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="16"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="21.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="9" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="21.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="16"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="21.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="9"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="9" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="21.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="16"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="21.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" ht="9" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="21.75" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="16"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="21.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="9" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="21.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="16"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="14"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="21.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="9"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="9" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="14"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="21.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="9"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="9" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="21.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="16"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="14"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="21.75" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="9"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="9" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="21.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="16"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="21.75" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="9"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="9" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="21.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="14"/>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="21.75" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="9"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="7"/>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="9" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="21.75" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="21.75" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="9"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="9" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="21.75" customHeight="1">
       <c r="A41" s="1"/>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="16"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="14"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="21.75" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="9"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="7"/>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="9" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="21.75" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="16"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="14"/>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="21.75" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="9"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="7"/>
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="9" customHeight="1">
       <c r="A46" s="1"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="21.75" customHeight="1">
       <c r="A47" s="1"/>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="16"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="21.75" customHeight="1">
       <c r="A48" s="1"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="9"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="7"/>
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="9" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="21.75" customHeight="1">
       <c r="A50" s="1"/>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="16"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="14"/>
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="21.75" customHeight="1">
       <c r="A51" s="1"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="9"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="7"/>
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="3.75" customHeight="1">

</xml_diff>